<commit_message>
# WARNING: head commit changed in the meantime
A
</commit_message>
<xml_diff>
--- a/SpiritZone/custom-reports/EXCEL-REPORT/21-Sep-2020.xlsx
+++ b/SpiritZone/custom-reports/EXCEL-REPORT/21-Sep-2020.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
   <si>
     <t>Pass</t>
   </si>
@@ -119,6 +119,15 @@
   </si>
   <si>
     <t>142.734</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>2020-09-21 22:38:22</t>
+  </si>
+  <si>
+    <t>74.569</t>
   </si>
 </sst>
 </file>
@@ -284,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -428,6 +437,36 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
@@ -1890,8 +1929,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="n" s="62">
-        <v>2.0</v>
+      <c r="A2" t="n" s="72">
+        <v>3.0</v>
       </c>
       <c r="B2" t="n" s="52">
         <v>3.0</v>
@@ -1899,8 +1938,8 @@
       <c r="C2" s="5">
         <v>0</v>
       </c>
-      <c r="D2" t="n" s="63">
-        <v>5.0</v>
+      <c r="D2" t="n" s="73">
+        <v>6.0</v>
       </c>
     </row>
   </sheetData>
@@ -1917,7 +1956,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2081,6 +2120,30 @@
       </c>
       <c r="H6" s="61"/>
     </row>
+    <row r="7">
+      <c r="A7" t="s" s="64">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s" s="65">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s" s="66">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s" s="67">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s" s="68">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s" s="69">
+        <v>35</v>
+      </c>
+      <c r="G7" t="s" s="70">
+        <v>17</v>
+      </c>
+      <c r="H7" s="71"/>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>